<commit_message>
Added place of birth to FU
</commit_message>
<xml_diff>
--- a/app/config/tables/PREGNANCIES/Forms/PREGNANCIES/PREGNANCIES.xlsx
+++ b/app/config/tables/PREGNANCIES/Forms/PREGNANCIES/PREGNANCIES.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D666402F-5669-4F37-8772-299E85492B58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BE93FE-6C56-467B-BEC7-A63CA1249F04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="274">
   <si>
     <t>setting_name</t>
   </si>
@@ -839,6 +839,24 @@
   </si>
   <si>
     <t>Tem cicatriz, não tenho certeza se BCG</t>
+  </si>
+  <si>
+    <t>regpar</t>
+  </si>
+  <si>
+    <t>select_one_dropdown</t>
+  </si>
+  <si>
+    <t>LOCPARCODE</t>
+  </si>
+  <si>
+    <t>locparcodens</t>
+  </si>
+  <si>
+    <t>select_multiple</t>
+  </si>
+  <si>
+    <t>LOCPAROU</t>
   </si>
 </sst>
 </file>
@@ -2651,7 +2669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
@@ -3846,9 +3864,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4253,7 +4271,7 @@
       <c r="A30" t="s">
         <v>166</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" t="s">
         <v>28</v>
       </c>
       <c r="C30" t="b">
@@ -4275,7 +4293,6 @@
       <c r="C31" t="b">
         <v>0</v>
       </c>
-      <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -4327,45 +4344,94 @@
       <c r="C35" t="b">
         <v>0</v>
       </c>
+      <c r="D35"/>
       <c r="E35"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>268</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>269</v>
       </c>
       <c r="C36" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D36"/>
       <c r="E36"/>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>167</v>
+        <v>270</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>269</v>
       </c>
       <c r="C37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>271</v>
+      </c>
+      <c r="B38" t="s">
+        <v>272</v>
+      </c>
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38"/>
+      <c r="G38"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>273</v>
+      </c>
+      <c r="B39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>167</v>
+      </c>
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>161</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B42" t="s">
         <v>48</v>
       </c>
-      <c r="C38" t="b">
-        <v>1</v>
-      </c>
-      <c r="G38"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C42" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42"/>
       <c r="G42"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>